<commit_message>
Added new subdivision, pipeline to process all objects in database, and function to save multiple histograms
</commit_message>
<xml_diff>
--- a/features/data.xlsx
+++ b/features/data.xlsx
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="I9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1161,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1593,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1665,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1773,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1806,7 +1806,7 @@
         </is>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="I39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         </is>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="I48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="b">
         <v>0</v>
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="I49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
@@ -2238,7 +2238,7 @@
         </is>
       </c>
       <c r="I50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="I51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="b">
         <v>0</v>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2346,7 +2346,7 @@
         </is>
       </c>
       <c r="I53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="I54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="b">
         <v>0</v>
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="I55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="b">
         <v>0</v>
@@ -2454,7 +2454,7 @@
         </is>
       </c>
       <c r="I56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="b">
         <v>0</v>
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="I58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="b">
         <v>0</v>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="b">
         <v>0</v>
@@ -2598,7 +2598,7 @@
         </is>
       </c>
       <c r="I60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="b">
         <v>0</v>
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="I61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="b">
         <v>0</v>
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="I62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" t="b">
         <v>0</v>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="J63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2850,7 +2850,7 @@
         </is>
       </c>
       <c r="I67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="b">
         <v>0</v>
@@ -2889,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="J68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="J69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2961,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="J70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2997,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="J71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3069,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="J73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="J74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="J75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="I76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76" t="b">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="J77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -3249,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="J78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="I79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="b">
         <v>0</v>
@@ -3318,7 +3318,7 @@
         </is>
       </c>
       <c r="I80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" t="b">
         <v>0</v>
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="I82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J82" t="b">
         <v>0</v>
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="I83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="b">
         <v>0</v>
@@ -3465,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="J84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -3501,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="J85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3534,7 +3534,7 @@
         </is>
       </c>
       <c r="I86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J86" t="b">
         <v>0</v>
@@ -3573,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="J87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -3606,7 +3606,7 @@
         </is>
       </c>
       <c r="I88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J88" t="b">
         <v>0</v>
@@ -3645,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="J89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -3681,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="J90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3717,7 +3717,7 @@
         <v>0</v>
       </c>
       <c r="J91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="J92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -3825,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="J94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="J95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3897,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="J96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -3933,7 +3933,7 @@
         <v>0</v>
       </c>
       <c r="J97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -3969,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="J98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="J101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="J102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -4146,7 +4146,7 @@
         </is>
       </c>
       <c r="I103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J103" t="b">
         <v>0</v>
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="J104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
       <c r="J105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -4254,7 +4254,7 @@
         </is>
       </c>
       <c r="I106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J106" t="b">
         <v>0</v>
@@ -4290,7 +4290,7 @@
         </is>
       </c>
       <c r="I107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J107" t="b">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="J109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -4398,7 +4398,7 @@
         </is>
       </c>
       <c r="I110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="b">
         <v>0</v>
@@ -4434,7 +4434,7 @@
         </is>
       </c>
       <c r="I111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" t="b">
         <v>0</v>
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="I112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J112" t="b">
         <v>0</v>
@@ -4509,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="J113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -4545,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="J114" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -4581,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="J115" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4617,7 +4617,7 @@
         <v>0</v>
       </c>
       <c r="J116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="I119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J119" t="b">
         <v>0</v>
@@ -4761,7 +4761,7 @@
         <v>0</v>
       </c>
       <c r="J120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4866,7 +4866,7 @@
         </is>
       </c>
       <c r="I123" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J123" t="b">
         <v>0</v>
@@ -4974,7 +4974,7 @@
         </is>
       </c>
       <c r="I126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J126" t="b">
         <v>0</v>
@@ -5049,7 +5049,7 @@
         <v>0</v>
       </c>
       <c r="J128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="I129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J129" t="b">
         <v>0</v>
@@ -5121,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="J130" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -5190,7 +5190,7 @@
         </is>
       </c>
       <c r="I132" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J132" t="b">
         <v>0</v>
@@ -5226,7 +5226,7 @@
         </is>
       </c>
       <c r="I133" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J133" t="b">
         <v>0</v>
@@ -5265,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="J134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -5298,7 +5298,7 @@
         </is>
       </c>
       <c r="I135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135" t="b">
         <v>0</v>
@@ -5337,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="J136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5373,7 +5373,7 @@
         <v>0</v>
       </c>
       <c r="J137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -5409,7 +5409,7 @@
         <v>0</v>
       </c>
       <c r="J138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -5442,7 +5442,7 @@
         </is>
       </c>
       <c r="I139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J139" t="b">
         <v>0</v>
@@ -5478,7 +5478,7 @@
         </is>
       </c>
       <c r="I140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J140" t="b">
         <v>0</v>
@@ -5514,7 +5514,7 @@
         </is>
       </c>
       <c r="I141" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J141" t="b">
         <v>0</v>
@@ -5550,7 +5550,7 @@
         </is>
       </c>
       <c r="I142" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J142" t="b">
         <v>0</v>
@@ -5589,7 +5589,7 @@
         <v>0</v>
       </c>
       <c r="J143" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -5625,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="J144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -5661,7 +5661,7 @@
         <v>0</v>
       </c>
       <c r="J145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -5694,7 +5694,7 @@
         </is>
       </c>
       <c r="I146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J146" t="b">
         <v>0</v>
@@ -5730,7 +5730,7 @@
         </is>
       </c>
       <c r="I147" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J147" t="b">
         <v>0</v>
@@ -5769,7 +5769,7 @@
         <v>0</v>
       </c>
       <c r="J148" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -5802,7 +5802,7 @@
         </is>
       </c>
       <c r="I149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J149" t="b">
         <v>0</v>
@@ -5841,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="J150" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="J151" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -5910,7 +5910,7 @@
         </is>
       </c>
       <c r="I152" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J152" t="b">
         <v>0</v>
@@ -5946,7 +5946,7 @@
         </is>
       </c>
       <c r="I153" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J153" t="b">
         <v>0</v>
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="I154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J154" t="b">
         <v>0</v>
@@ -6021,7 +6021,7 @@
         <v>0</v>
       </c>
       <c r="J155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -6057,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="J156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -6090,7 +6090,7 @@
         </is>
       </c>
       <c r="I157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J157" t="b">
         <v>0</v>
@@ -6129,7 +6129,7 @@
         <v>0</v>
       </c>
       <c r="J158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -6165,7 +6165,7 @@
         <v>0</v>
       </c>
       <c r="J159" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="J161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -6273,7 +6273,7 @@
         <v>0</v>
       </c>
       <c r="J162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -6309,7 +6309,7 @@
         <v>0</v>
       </c>
       <c r="J163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -6345,7 +6345,7 @@
         <v>0</v>
       </c>
       <c r="J164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -6381,7 +6381,7 @@
         <v>0</v>
       </c>
       <c r="J165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -6417,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="J166" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -6453,7 +6453,7 @@
         <v>0</v>
       </c>
       <c r="J167" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -6489,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="J168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -6525,7 +6525,7 @@
         <v>0</v>
       </c>
       <c r="J169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -6558,7 +6558,7 @@
         </is>
       </c>
       <c r="I170" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J170" t="b">
         <v>0</v>
@@ -6597,7 +6597,7 @@
         <v>0</v>
       </c>
       <c r="J171" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="J172" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -6705,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="J174" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -6741,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="J175" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -6777,7 +6777,7 @@
         <v>0</v>
       </c>
       <c r="J176" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -6810,7 +6810,7 @@
         </is>
       </c>
       <c r="I177" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J177" t="b">
         <v>0</v>
@@ -6849,7 +6849,7 @@
         <v>0</v>
       </c>
       <c r="J178" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -6885,7 +6885,7 @@
         <v>0</v>
       </c>
       <c r="J179" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -6921,7 +6921,7 @@
         <v>0</v>
       </c>
       <c r="J180" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -6957,7 +6957,7 @@
         <v>0</v>
       </c>
       <c r="J181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -7065,7 +7065,7 @@
         <v>0</v>
       </c>
       <c r="J184" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -7098,7 +7098,7 @@
         </is>
       </c>
       <c r="I185" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J185" t="b">
         <v>0</v>
@@ -7134,7 +7134,7 @@
         </is>
       </c>
       <c r="I186" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J186" t="b">
         <v>0</v>
@@ -7173,7 +7173,7 @@
         <v>0</v>
       </c>
       <c r="J187" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -7209,7 +7209,7 @@
         <v>0</v>
       </c>
       <c r="J188" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -7245,7 +7245,7 @@
         <v>0</v>
       </c>
       <c r="J189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -7281,7 +7281,7 @@
         <v>0</v>
       </c>
       <c r="J190" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -7317,7 +7317,7 @@
         <v>0</v>
       </c>
       <c r="J191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -7353,7 +7353,7 @@
         <v>0</v>
       </c>
       <c r="J192" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
@@ -7389,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="J193" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -7422,7 +7422,7 @@
         </is>
       </c>
       <c r="I194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J194" t="b">
         <v>0</v>
@@ -7533,7 +7533,7 @@
         <v>0</v>
       </c>
       <c r="J197" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -7569,7 +7569,7 @@
         <v>0</v>
       </c>
       <c r="J198" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -7602,7 +7602,7 @@
         </is>
       </c>
       <c r="I199" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J199" t="b">
         <v>0</v>
@@ -7641,7 +7641,7 @@
         <v>0</v>
       </c>
       <c r="J200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -7674,7 +7674,7 @@
         </is>
       </c>
       <c r="I201" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J201" t="b">
         <v>0</v>
@@ -7749,7 +7749,7 @@
         <v>0</v>
       </c>
       <c r="J203" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="I204" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J204" t="b">
         <v>0</v>
@@ -7821,7 +7821,7 @@
         <v>0</v>
       </c>
       <c r="J205" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -7857,7 +7857,7 @@
         <v>0</v>
       </c>
       <c r="J206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -7926,7 +7926,7 @@
         </is>
       </c>
       <c r="I208" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J208" t="b">
         <v>0</v>
@@ -7962,7 +7962,7 @@
         </is>
       </c>
       <c r="I209" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J209" t="b">
         <v>0</v>
@@ -8001,7 +8001,7 @@
         <v>0</v>
       </c>
       <c r="J210" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -8037,7 +8037,7 @@
         <v>0</v>
       </c>
       <c r="J211" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -8070,7 +8070,7 @@
         </is>
       </c>
       <c r="I212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J212" t="b">
         <v>0</v>
@@ -8106,7 +8106,7 @@
         </is>
       </c>
       <c r="I213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J213" t="b">
         <v>0</v>
@@ -8145,7 +8145,7 @@
         <v>0</v>
       </c>
       <c r="J214" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -8181,7 +8181,7 @@
         <v>0</v>
       </c>
       <c r="J215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">
@@ -8217,7 +8217,7 @@
         <v>0</v>
       </c>
       <c r="J216" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -8253,7 +8253,7 @@
         <v>0</v>
       </c>
       <c r="J217" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -8289,7 +8289,7 @@
         <v>0</v>
       </c>
       <c r="J218" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -8325,7 +8325,7 @@
         <v>0</v>
       </c>
       <c r="J219" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -8361,7 +8361,7 @@
         <v>0</v>
       </c>
       <c r="J220" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -8397,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="J221" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -8430,7 +8430,7 @@
         </is>
       </c>
       <c r="I222" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J222" t="b">
         <v>0</v>
@@ -8469,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="J223" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -8502,7 +8502,7 @@
         </is>
       </c>
       <c r="I224" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J224" t="b">
         <v>0</v>
@@ -8541,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="J225" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -8574,7 +8574,7 @@
         </is>
       </c>
       <c r="I226" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J226" t="b">
         <v>0</v>
@@ -8610,7 +8610,7 @@
         </is>
       </c>
       <c r="I227" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J227" t="b">
         <v>0</v>
@@ -8646,7 +8646,7 @@
         </is>
       </c>
       <c r="I228" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J228" t="b">
         <v>0</v>
@@ -8682,7 +8682,7 @@
         </is>
       </c>
       <c r="I229" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J229" t="b">
         <v>0</v>
@@ -8718,7 +8718,7 @@
         </is>
       </c>
       <c r="I230" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J230" t="b">
         <v>0</v>
@@ -8754,7 +8754,7 @@
         </is>
       </c>
       <c r="I231" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J231" t="b">
         <v>0</v>
@@ -8790,7 +8790,7 @@
         </is>
       </c>
       <c r="I232" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J232" t="b">
         <v>0</v>
@@ -8826,7 +8826,7 @@
         </is>
       </c>
       <c r="I233" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J233" t="b">
         <v>0</v>
@@ -8862,7 +8862,7 @@
         </is>
       </c>
       <c r="I234" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J234" t="b">
         <v>0</v>
@@ -8898,7 +8898,7 @@
         </is>
       </c>
       <c r="I235" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J235" t="b">
         <v>0</v>
@@ -8934,7 +8934,7 @@
         </is>
       </c>
       <c r="I236" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J236" t="b">
         <v>0</v>
@@ -8970,7 +8970,7 @@
         </is>
       </c>
       <c r="I237" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J237" t="b">
         <v>0</v>
@@ -9042,7 +9042,7 @@
         </is>
       </c>
       <c r="I239" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J239" t="b">
         <v>0</v>
@@ -9114,7 +9114,7 @@
         </is>
       </c>
       <c r="I241" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J241" t="b">
         <v>0</v>
@@ -9150,7 +9150,7 @@
         </is>
       </c>
       <c r="I242" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J242" t="b">
         <v>0</v>
@@ -9186,7 +9186,7 @@
         </is>
       </c>
       <c r="I243" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J243" t="b">
         <v>0</v>
@@ -9225,7 +9225,7 @@
         <v>0</v>
       </c>
       <c r="J244" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -9258,7 +9258,7 @@
         </is>
       </c>
       <c r="I245" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J245" t="b">
         <v>0</v>

</xml_diff>